<commit_message>
1st stability check done
</commit_message>
<xml_diff>
--- a/data/email_list.xlsx
+++ b/data/email_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\coding\WahyzAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F887FA6-A1AB-4815-A913-1CC7E48527B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228E7B79-647A-41DE-A7C3-7873C706F5F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13350" yWindow="2295" windowWidth="14790" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="615" yWindow="12750" windowWidth="12150" windowHeight="11520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -41,31 +41,45 @@
   </si>
   <si>
     <t>Number</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ksyoon568@naver.com</t>
+  </si>
+  <si>
+    <t>ksyoon568@gmail.com</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ksyoon_naver</t>
+  </si>
+  <si>
+    <t>ksyoon_gmail</t>
+  </si>
+  <si>
+    <t>330(2)</t>
+  </si>
+  <si>
+    <t>2(2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -79,14 +93,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -98,14 +105,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -408,51 +412,94 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1">
       <c r="A1" t="s">
         <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="21" customHeight="1">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2">
+        <v>330</v>
+      </c>
+      <c r="C2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="21" customHeight="1">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{FDCEC46D-391A-4928-A6B5-B0A1D42B5926}"/>
+    <hyperlink ref="D5" r:id="rId2" xr:uid="{6570F019-6C40-4CB8-988A-090BB810941B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>